<commit_message>
Modify notebook and initial execution of optimisation with results
</commit_message>
<xml_diff>
--- a/Src/Results_insertion/output_insertion_high_[0, 2]_0.xlsx
+++ b/Src/Results_insertion/output_insertion_high_[0, 2]_0.xlsx
@@ -789,7 +789,7 @@
         <v>4</v>
       </c>
       <c r="O7" t="n">
-        <v>0.006113767623901367</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -836,7 +836,7 @@
         <v>5</v>
       </c>
       <c r="O8" t="n">
-        <v>0.006941318511962891</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -977,7 +977,7 @@
         <v>6</v>
       </c>
       <c r="O11" t="n">
-        <v>0.01565074920654297</v>
+        <v>0.01579952239990234</v>
       </c>
     </row>
     <row r="12">
@@ -1024,7 +1024,7 @@
         <v>5</v>
       </c>
       <c r="O12" t="n">
-        <v>0.01119518280029297</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -1118,7 +1118,7 @@
         <v>6</v>
       </c>
       <c r="O14" t="n">
-        <v>0.5646049976348877</v>
+        <v>0.149911642074585</v>
       </c>
     </row>
     <row r="15">
@@ -1165,7 +1165,7 @@
         <v>7</v>
       </c>
       <c r="O15" t="n">
-        <v>0</v>
+        <v>0.001105308532714844</v>
       </c>
     </row>
     <row r="16">
@@ -1259,7 +1259,7 @@
         <v>8</v>
       </c>
       <c r="O17" t="n">
-        <v>0.003033876419067383</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -1353,7 +1353,7 @@
         <v>8</v>
       </c>
       <c r="O19" t="n">
-        <v>0.01643824577331543</v>
+        <v>0.005612611770629883</v>
       </c>
     </row>
     <row r="20">
@@ -1400,7 +1400,7 @@
         <v>7</v>
       </c>
       <c r="O20" t="n">
-        <v>0.01578354835510254</v>
+        <v>0.001584529876708984</v>
       </c>
     </row>
     <row r="21">
@@ -1447,7 +1447,7 @@
         <v>8</v>
       </c>
       <c r="O21" t="n">
-        <v>0.009863138198852539</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1635,7 +1635,7 @@
         <v>10</v>
       </c>
       <c r="O25" t="n">
-        <v>0.01706910133361816</v>
+        <v>0.006570339202880859</v>
       </c>
     </row>
     <row r="26">
@@ -1682,7 +1682,7 @@
         <v>10</v>
       </c>
       <c r="O26" t="n">
-        <v>0.1609432697296143</v>
+        <v>0.05611276626586914</v>
       </c>
     </row>
     <row r="27">
@@ -1729,7 +1729,7 @@
         <v>11</v>
       </c>
       <c r="O27" t="n">
-        <v>0.0101618766784668</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -1823,7 +1823,7 @@
         <v>12</v>
       </c>
       <c r="O29" t="n">
-        <v>0.01564836502075195</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1870,7 +1870,7 @@
         <v>11</v>
       </c>
       <c r="O30" t="n">
-        <v>0.001531600952148438</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -1917,7 +1917,7 @@
         <v>12</v>
       </c>
       <c r="O31" t="n">
-        <v>0.008037090301513672</v>
+        <v>0.004039764404296875</v>
       </c>
     </row>
     <row r="32">
@@ -2011,7 +2011,7 @@
         <v>14</v>
       </c>
       <c r="O33" t="n">
-        <v>0.01565837860107422</v>
+        <v>0.01628589630126953</v>
       </c>
     </row>
     <row r="34">
@@ -2058,7 +2058,7 @@
         <v>16</v>
       </c>
       <c r="O34" t="n">
-        <v>0.4829103946685791</v>
+        <v>0.08252167701721191</v>
       </c>
     </row>
     <row r="35">
@@ -2105,7 +2105,7 @@
         <v>17</v>
       </c>
       <c r="O35" t="n">
-        <v>0.1483852863311768</v>
+        <v>0.03958797454833984</v>
       </c>
     </row>
     <row r="36">
@@ -2152,7 +2152,7 @@
         <v>17</v>
       </c>
       <c r="O36" t="n">
-        <v>0.008520126342773438</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -2199,7 +2199,7 @@
         <v>19</v>
       </c>
       <c r="O37" t="n">
-        <v>0.9539873600006104</v>
+        <v>0.3334903717041016</v>
       </c>
     </row>
     <row r="38">
@@ -2246,7 +2246,7 @@
         <v>20</v>
       </c>
       <c r="O38" t="n">
-        <v>0.0101315975189209</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -2293,7 +2293,7 @@
         <v>20</v>
       </c>
       <c r="O39" t="n">
-        <v>0.01564383506774902</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -2340,7 +2340,7 @@
         <v>19</v>
       </c>
       <c r="O40" t="n">
-        <v>0.01402139663696289</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -2387,7 +2387,7 @@
         <v>20</v>
       </c>
       <c r="O41" t="n">
-        <v>0.006796121597290039</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -2434,7 +2434,7 @@
         <v>21</v>
       </c>
       <c r="O42" t="n">
-        <v>0.003371238708496094</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -2481,7 +2481,7 @@
         <v>22</v>
       </c>
       <c r="O43" t="n">
-        <v>0.008534431457519531</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -2528,7 +2528,7 @@
         <v>22</v>
       </c>
       <c r="O44" t="n">
-        <v>0.0100102424621582</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -2622,7 +2622,7 @@
         <v>19</v>
       </c>
       <c r="O46" t="n">
-        <v>0.00948333740234375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -2669,7 +2669,7 @@
         <v>20</v>
       </c>
       <c r="O47" t="n">
-        <v>0.03136277198791504</v>
+        <v>0.007104396820068359</v>
       </c>
     </row>
     <row r="48">
@@ -2716,7 +2716,7 @@
         <v>21</v>
       </c>
       <c r="O48" t="n">
-        <v>0.01352596282958984</v>
+        <v>0.001598119735717773</v>
       </c>
     </row>
     <row r="49">
@@ -2763,7 +2763,7 @@
         <v>22</v>
       </c>
       <c r="O49" t="n">
-        <v>0.0194704532623291</v>
+        <v>0.007414340972900391</v>
       </c>
     </row>
     <row r="50">
@@ -2810,7 +2810,7 @@
         <v>19</v>
       </c>
       <c r="O50" t="n">
-        <v>0.01206851005554199</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -2904,7 +2904,7 @@
         <v>18</v>
       </c>
       <c r="O52" t="n">
-        <v>0.002757787704467773</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -2951,7 +2951,7 @@
         <v>19</v>
       </c>
       <c r="O53" t="n">
-        <v>0.01795148849487305</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -2998,7 +2998,7 @@
         <v>17</v>
       </c>
       <c r="O54" t="n">
-        <v>0.01555323600769043</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -3045,7 +3045,7 @@
         <v>17</v>
       </c>
       <c r="O55" t="n">
-        <v>0.02004361152648926</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -3092,7 +3092,7 @@
         <v>13</v>
       </c>
       <c r="O56" t="n">
-        <v>0.005414962768554688</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -3139,7 +3139,7 @@
         <v>14</v>
       </c>
       <c r="O57" t="n">
-        <v>0.01572632789611816</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -3233,7 +3233,7 @@
         <v>12</v>
       </c>
       <c r="O59" t="n">
-        <v>0.01602649688720703</v>
+        <v>0.0101008415222168</v>
       </c>
     </row>
     <row r="60">
@@ -3280,7 +3280,7 @@
         <v>13</v>
       </c>
       <c r="O60" t="n">
-        <v>0.0271759033203125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -3327,7 +3327,7 @@
         <v>14</v>
       </c>
       <c r="O61" t="n">
-        <v>0</v>
+        <v>0.01000475883483887</v>
       </c>
     </row>
     <row r="62">
@@ -3374,7 +3374,7 @@
         <v>15</v>
       </c>
       <c r="O62" t="n">
-        <v>0.01170897483825684</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -3421,7 +3421,7 @@
         <v>16</v>
       </c>
       <c r="O63" t="n">
-        <v>0.002020120620727539</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -3468,7 +3468,7 @@
         <v>16</v>
       </c>
       <c r="O64" t="n">
-        <v>0.06388235092163086</v>
+        <v>0.01572990417480469</v>
       </c>
     </row>
     <row r="65">
@@ -3515,7 +3515,7 @@
         <v>13</v>
       </c>
       <c r="O65" t="n">
-        <v>1.543753385543823</v>
+        <v>0.460355281829834</v>
       </c>
     </row>
     <row r="66">
@@ -3562,7 +3562,7 @@
         <v>14</v>
       </c>
       <c r="O66" t="n">
-        <v>0.005511999130249023</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -3609,7 +3609,7 @@
         <v>15</v>
       </c>
       <c r="O67" t="n">
-        <v>0.01572680473327637</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -3656,7 +3656,7 @@
         <v>11</v>
       </c>
       <c r="O68" t="n">
-        <v>0.01001691818237305</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -3703,7 +3703,7 @@
         <v>12</v>
       </c>
       <c r="O69" t="n">
-        <v>0.08703804016113281</v>
+        <v>0.01071667671203613</v>
       </c>
     </row>
     <row r="70">
@@ -3797,7 +3797,7 @@
         <v>14</v>
       </c>
       <c r="O71" t="n">
-        <v>5.07501220703125</v>
+        <v>1.78434681892395</v>
       </c>
     </row>
     <row r="72">
@@ -3844,7 +3844,7 @@
         <v>17</v>
       </c>
       <c r="O72" t="n">
-        <v>22.38944268226624</v>
+        <v>17.63679718971252</v>
       </c>
     </row>
     <row r="73">
@@ -3891,7 +3891,7 @@
         <v>12</v>
       </c>
       <c r="O73" t="n">
-        <v>0.03359460830688477</v>
+        <v>0.0271143913269043</v>
       </c>
     </row>
     <row r="74">
@@ -3985,7 +3985,7 @@
         <v>11</v>
       </c>
       <c r="O75" t="n">
-        <v>0</v>
+        <v>0.001001834869384766</v>
       </c>
     </row>
     <row r="76">
@@ -4079,7 +4079,7 @@
         <v>12</v>
       </c>
       <c r="O77" t="n">
-        <v>0.001004695892333984</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -4126,7 +4126,7 @@
         <v>13</v>
       </c>
       <c r="O78" t="n">
-        <v>0</v>
+        <v>0.01403594017028809</v>
       </c>
     </row>
     <row r="79">
@@ -4173,7 +4173,7 @@
         <v>14</v>
       </c>
       <c r="O79" t="n">
-        <v>0.007747650146484375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80">
@@ -4220,7 +4220,7 @@
         <v>14</v>
       </c>
       <c r="O80" t="n">
-        <v>0</v>
+        <v>0.001890659332275391</v>
       </c>
     </row>
     <row r="81">
@@ -4267,7 +4267,7 @@
         <v>15</v>
       </c>
       <c r="O81" t="n">
-        <v>0.07436132431030273</v>
+        <v>0.08059287071228027</v>
       </c>
     </row>
     <row r="82">
@@ -4408,7 +4408,7 @@
         <v>17</v>
       </c>
       <c r="O84" t="n">
-        <v>3.48161792755127</v>
+        <v>4.013778209686279</v>
       </c>
     </row>
     <row r="85">
@@ -4455,7 +4455,7 @@
         <v>16</v>
       </c>
       <c r="O85" t="n">
-        <v>0</v>
+        <v>0.006505250930786133</v>
       </c>
     </row>
     <row r="86">
@@ -4549,7 +4549,7 @@
         <v>16</v>
       </c>
       <c r="O87" t="n">
-        <v>0.04154324531555176</v>
+        <v>0.04182934761047363</v>
       </c>
     </row>
     <row r="88">
@@ -4596,7 +4596,7 @@
         <v>16</v>
       </c>
       <c r="O88" t="n">
-        <v>0.0380854606628418</v>
+        <v>0.04611086845397949</v>
       </c>
     </row>
     <row r="89">
@@ -4643,7 +4643,7 @@
         <v>17</v>
       </c>
       <c r="O89" t="n">
-        <v>0.0161283016204834</v>
+        <v>0.0009243488311767578</v>
       </c>
     </row>
     <row r="90">
@@ -4690,7 +4690,7 @@
         <v>18</v>
       </c>
       <c r="O90" t="n">
-        <v>0.06776332855224609</v>
+        <v>0.06563925743103027</v>
       </c>
     </row>
     <row r="91">
@@ -4737,7 +4737,7 @@
         <v>16</v>
       </c>
       <c r="O91" t="n">
-        <v>0.01165676116943359</v>
+        <v>0.03500270843505859</v>
       </c>
     </row>
     <row r="92">
@@ -4784,7 +4784,7 @@
         <v>17</v>
       </c>
       <c r="O92" t="n">
-        <v>0.01590991020202637</v>
+        <v>0.02590513229370117</v>
       </c>
     </row>
     <row r="93">
@@ -4831,7 +4831,7 @@
         <v>16</v>
       </c>
       <c r="O93" t="n">
-        <v>0.04645514488220215</v>
+        <v>0.04880595207214355</v>
       </c>
     </row>
     <row r="94">
@@ -4878,7 +4878,7 @@
         <v>14</v>
       </c>
       <c r="O94" t="n">
-        <v>0.03084969520568848</v>
+        <v>0.0333554744720459</v>
       </c>
     </row>
     <row r="95">
@@ -4925,7 +4925,7 @@
         <v>14</v>
       </c>
       <c r="O95" t="n">
-        <v>0.0391545295715332</v>
+        <v>0.0481259822845459</v>
       </c>
     </row>
     <row r="96">
@@ -4972,7 +4972,7 @@
         <v>16</v>
       </c>
       <c r="O96" t="n">
-        <v>0.03989934921264648</v>
+        <v>0.03818821907043457</v>
       </c>
     </row>
     <row r="97">
@@ -5066,7 +5066,7 @@
         <v>18</v>
       </c>
       <c r="O98" t="n">
-        <v>0.02473974227905273</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99">
@@ -5113,7 +5113,7 @@
         <v>19</v>
       </c>
       <c r="O99" t="n">
-        <v>0.0164189338684082</v>
+        <v>0.0270392894744873</v>
       </c>
     </row>
     <row r="100">
@@ -5160,7 +5160,7 @@
         <v>17</v>
       </c>
       <c r="O100" t="n">
-        <v>0.002171754837036133</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101">
@@ -5207,7 +5207,7 @@
         <v>18</v>
       </c>
       <c r="O101" t="n">
-        <v>0.01538920402526855</v>
+        <v>0.01790833473205566</v>
       </c>
     </row>
     <row r="102">
@@ -5254,7 +5254,7 @@
         <v>19</v>
       </c>
       <c r="O102" t="n">
-        <v>0.03569149971008301</v>
+        <v>0.04964923858642578</v>
       </c>
     </row>
     <row r="103">
@@ -5301,7 +5301,7 @@
         <v>18</v>
       </c>
       <c r="O103" t="n">
-        <v>0.005506277084350586</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104">
@@ -5348,7 +5348,7 @@
         <v>20</v>
       </c>
       <c r="O104" t="n">
-        <v>0.648249626159668</v>
+        <v>0.9572534561157227</v>
       </c>
     </row>
     <row r="105">
@@ -5442,7 +5442,7 @@
         <v>22</v>
       </c>
       <c r="O106" t="n">
-        <v>0</v>
+        <v>0.02267694473266602</v>
       </c>
     </row>
     <row r="107">
@@ -5536,7 +5536,7 @@
         <v>24</v>
       </c>
       <c r="O108" t="n">
-        <v>0</v>
+        <v>0.01648998260498047</v>
       </c>
     </row>
     <row r="109">
@@ -5583,7 +5583,7 @@
         <v>25</v>
       </c>
       <c r="O109" t="n">
-        <v>0.01573801040649414</v>
+        <v>0.007256031036376953</v>
       </c>
     </row>
     <row r="110">
@@ -5630,7 +5630,7 @@
         <v>22</v>
       </c>
       <c r="O110" t="n">
-        <v>0</v>
+        <v>0.01356053352355957</v>
       </c>
     </row>
     <row r="111">
@@ -5677,7 +5677,7 @@
         <v>23</v>
       </c>
       <c r="O111" t="n">
-        <v>0.04742193222045898</v>
+        <v>0.06697845458984375</v>
       </c>
     </row>
     <row r="112">
@@ -5724,7 +5724,7 @@
         <v>23</v>
       </c>
       <c r="O112" t="n">
-        <v>0.08128952980041504</v>
+        <v>0.09998917579650879</v>
       </c>
     </row>
     <row r="113">
@@ -5771,7 +5771,7 @@
         <v>23</v>
       </c>
       <c r="O113" t="n">
-        <v>0.06788134574890137</v>
+        <v>0.09976100921630859</v>
       </c>
     </row>
     <row r="114">
@@ -5818,7 +5818,7 @@
         <v>23</v>
       </c>
       <c r="O114" t="n">
-        <v>0.08984112739562988</v>
+        <v>0.08468890190124512</v>
       </c>
     </row>
     <row r="115">
@@ -5865,7 +5865,7 @@
         <v>19</v>
       </c>
       <c r="O115" t="n">
-        <v>0.001581430435180664</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116">
@@ -5912,7 +5912,7 @@
         <v>15</v>
       </c>
       <c r="O116" t="n">
-        <v>0.02020597457885742</v>
+        <v>0.04265499114990234</v>
       </c>
     </row>
     <row r="117">
@@ -6194,7 +6194,7 @@
         <v>13</v>
       </c>
       <c r="O122" t="n">
-        <v>0</v>
+        <v>0.01349592208862305</v>
       </c>
     </row>
     <row r="123">
@@ -6241,7 +6241,7 @@
         <v>8</v>
       </c>
       <c r="O123" t="n">
-        <v>0</v>
+        <v>0.00901484489440918</v>
       </c>
     </row>
     <row r="124">
@@ -6523,7 +6523,7 @@
         <v>6</v>
       </c>
       <c r="O129" t="n">
-        <v>0.0009839534759521484</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130">
@@ -6570,7 +6570,7 @@
         <v>5</v>
       </c>
       <c r="O130" t="n">
-        <v>0.001142978668212891</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131">
@@ -6711,7 +6711,7 @@
         <v>7</v>
       </c>
       <c r="O133" t="n">
-        <v>0.008607149124145508</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134">
@@ -6852,7 +6852,7 @@
         <v>6</v>
       </c>
       <c r="O136" t="n">
-        <v>0</v>
+        <v>0.0009992122650146484</v>
       </c>
     </row>
     <row r="137">
@@ -6946,7 +6946,7 @@
         <v>8</v>
       </c>
       <c r="O138" t="n">
-        <v>0</v>
+        <v>0.01255631446838379</v>
       </c>
     </row>
     <row r="139">
@@ -7040,7 +7040,7 @@
         <v>8</v>
       </c>
       <c r="O140" t="n">
-        <v>0</v>
+        <v>0.00130915641784668</v>
       </c>
     </row>
     <row r="141">
@@ -7181,7 +7181,7 @@
         <v>10</v>
       </c>
       <c r="O143" t="n">
-        <v>0.002005815505981445</v>
+        <v>0.004910469055175781</v>
       </c>
     </row>
     <row r="144">
@@ -7228,7 +7228,7 @@
         <v>11</v>
       </c>
       <c r="O144" t="n">
-        <v>0.0004525184631347656</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145">
@@ -7275,7 +7275,7 @@
         <v>12</v>
       </c>
       <c r="O145" t="n">
-        <v>0</v>
+        <v>0.001509666442871094</v>
       </c>
     </row>
     <row r="146">
@@ -7322,7 +7322,7 @@
         <v>11</v>
       </c>
       <c r="O146" t="n">
-        <v>0.0009996891021728516</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147">
@@ -7369,7 +7369,7 @@
         <v>12</v>
       </c>
       <c r="O147" t="n">
-        <v>0</v>
+        <v>0.001042842864990234</v>
       </c>
     </row>
     <row r="148">
@@ -7416,7 +7416,7 @@
         <v>12</v>
       </c>
       <c r="O148" t="n">
-        <v>0.01011395454406738</v>
+        <v>0.01930880546569824</v>
       </c>
     </row>
     <row r="149">
@@ -7463,7 +7463,7 @@
         <v>12</v>
       </c>
       <c r="O149" t="n">
-        <v>0.01568174362182617</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150">
@@ -7510,7 +7510,7 @@
         <v>7</v>
       </c>
       <c r="O150" t="n">
-        <v>0.2165226936340332</v>
+        <v>0.2493259906768799</v>
       </c>
     </row>
     <row r="151">
@@ -7557,7 +7557,7 @@
         <v>7</v>
       </c>
       <c r="O151" t="n">
-        <v>0.02018308639526367</v>
+        <v>0.02045822143554688</v>
       </c>
     </row>
     <row r="152">
@@ -7604,7 +7604,7 @@
         <v>6</v>
       </c>
       <c r="O152" t="n">
-        <v>0</v>
+        <v>0.009504556655883789</v>
       </c>
     </row>
     <row r="153">
@@ -8074,7 +8074,7 @@
         <v>4</v>
       </c>
       <c r="O162" t="n">
-        <v>0</v>
+        <v>0.004445791244506836</v>
       </c>
     </row>
     <row r="163">
@@ -8121,7 +8121,7 @@
         <v>5</v>
       </c>
       <c r="O163" t="n">
-        <v>0</v>
+        <v>0.0009999275207519531</v>
       </c>
     </row>
     <row r="164">
@@ -8215,7 +8215,7 @@
         <v>7</v>
       </c>
       <c r="O165" t="n">
-        <v>0</v>
+        <v>0.003006935119628906</v>
       </c>
     </row>
     <row r="166">
@@ -8356,7 +8356,7 @@
         <v>4</v>
       </c>
       <c r="O168" t="n">
-        <v>0</v>
+        <v>0.008615970611572266</v>
       </c>
     </row>
     <row r="169">
@@ -8450,7 +8450,7 @@
         <v>5</v>
       </c>
       <c r="O170" t="n">
-        <v>0.01918959617614746</v>
+        <v>0.01304388046264648</v>
       </c>
     </row>
     <row r="171">
@@ -8497,7 +8497,7 @@
         <v>5</v>
       </c>
       <c r="O171" t="n">
-        <v>0.005089998245239258</v>
+        <v>0.01666164398193359</v>
       </c>
     </row>
     <row r="172">
@@ -8638,7 +8638,7 @@
         <v>5</v>
       </c>
       <c r="O174" t="n">
-        <v>0.003905296325683594</v>
+        <v>0.01603484153747559</v>
       </c>
     </row>
     <row r="175">
@@ -8732,7 +8732,7 @@
         <v>4</v>
       </c>
       <c r="O176" t="n">
-        <v>0.001188755035400391</v>
+        <v>0</v>
       </c>
     </row>
     <row r="177">

</xml_diff>